<commit_message>
Upgrade bequeath-your-data-and-die forwarding, code updated for other comments
</commit_message>
<xml_diff>
--- a/testing/AA-v1+testcase.docs.xlsx
+++ b/testing/AA-v1+testcase.docs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\Documents\MW\MW-Germany\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW\AdministratorAdministration\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E11B494-7337-451A-88F9-989A74E9C941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA27C66-C91A-47FA-A8AA-78B360C58FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="161">
   <si>
     <t>Testcases</t>
   </si>
@@ -958,6 +958,21 @@
      - other attributes according to chosen http-c
      - operation-key from above
    - all parameters with realistic values (incl. DummyXCorrelator)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### Testing:
+- Checking for response-code 200
+- Extract applicationName, releaseNumber, address, protocol and port from output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals and store it in expectedApplicationsList.
+- Generate schema based on the specification
+- Checking the response body for each attribute against the generated schema
+- Checking the response body attributes against expectedApplicationsList.
+</t>
+  </si>
+  <si>
+    <t>Request body Attribute correctness?</t>
+  </si>
+  <si>
+    <t>Forwardings triggered?</t>
   </si>
 </sst>
 </file>
@@ -1385,10 +1400,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1713,10 +1728,10 @@
   <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomRight" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1868,6 +1883,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key
 - randomly choosing http-c from ltpList
+- Extracting authorization from config file
 ")
 &amp;CONCATENATE("
   - POST ",G3,"
@@ -1878,6 +1894,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
@@ -1907,13 +1924,15 @@
 - checking for ResponseCode==204 (not 400 because of idempotence)
 </v>
       </c>
-      <c r="F6" s="23" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G6" s="23" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="F6" s="23" t="str">
+        <f ca="1">$D6</f>
+        <v>#### Testing:
+- checking for ResponseCode==200</v>
+      </c>
+      <c r="G6" s="23" t="str">
+        <f ca="1">$D6</f>
+        <v>#### Testing:
+- checking for ResponseCode==200</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -1985,7 +2004,7 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",D$3,", storing operation-key
--  searching CC for output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals, find corresponding op-c, http-c and tcp-c, store them")
+-  searching CC for output fc-port of E9, find corresponding op-c, http-c and tcp-c, store them")
 &amp;CONCATENATE("
   - POST ",D$3,"
      - all attributes according to chosen http-c, tcp-c
@@ -1994,7 +2013,7 @@
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/regard-application, storing operation-key
--  searching CC for output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals, find corresponding op-c, http-c and tcp-c, store them
+-  searching CC for output fc-port of E9, find corresponding op-c, http-c and tcp-c, store them
   - POST /v1/regard-application
      - all attributes according to chosen http-c, tcp-c
     -operation-key from above
@@ -2037,19 +2056,19 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList")
+- Extracting authorization from config file")
 &amp;CONCATENATE("
-  - POST ",G3,"
-   - all attributes filled with chosen http-c and admin-p with method=GET
+ - POST ",G3,"
+   - all attributes filled with chosen http-c with method=GET
     -operation-key from above
     -  BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
-  - POST /v1/approve-oam-request
-   - all attributes filled with chosen http-c and admin-p with method=GET
+- Extracting authorization from config file
+ - POST /v1/approve-oam-request
+   - all attributes filled with chosen http-c with method=GET
     -operation-key from above
     -  BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)</v>
       </c>
@@ -2208,19 +2227,19 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList")
+- Extracting authorization from config file")
 &amp;CONCATENATE("
   - POST ",G$3,"
-    - all attributes filled with chosen http-c and admin-p with method=GET
+    - all attributes filled with chosen http-c with method=GET
      - all parameters with realistic values, BUT 
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
-    - all attributes filled with chosen http-c and admin-p with method=GET
+    - all attributes filled with chosen http-c with method=GET
      - all parameters with realistic values, BUT 
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).</v>
       </c>
@@ -2379,19 +2398,19 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList")
+- Extracting authorization from config file")
 &amp;CONCATENATE("
   - POST ",G$3,"
-    - all attributes filled with chosen http-c and admin-p with method=GET
+    - all attributes filled with chosen http-c with method=GET
     -operation-key from above
    - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
-    - all attributes filled with chosen http-c and admin-p with method=GET
+    - all attributes filled with chosen http-c with method=GET
     -operation-key from above
    - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)</v>
       </c>
@@ -2550,19 +2569,19 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList")
+- Extracting authorization from config file")
 &amp;CONCATENATE("
   - POST ",G$3,"
-    - all attributes filled with chosen http-c and admin-p with method=GET
+    - all attributes filled with chosen http-c with method=GET
     -operation-key from above
    - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
-    - all attributes filled with chosen http-c and admin-p with method=GET
+    - all attributes filled with chosen http-c with method=GET
     -operation-key from above
    - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)</v>
       </c>
@@ -2711,19 +2730,19 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList")
+- Extracting authorization from config file")
 &amp;CONCATENATE("
   - POST ",G$3,"
-     - all attributes filled with chosen http-c and admin-p with method=GET
+     - all attributes filled with chosen http-c with method=GET
      - reasonable parameters
     - BUT operationKey parameter missing (does not mean empty string)""")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
-     - all attributes filled with chosen http-c and admin-p with method=GET
+     - all attributes filled with chosen http-c with method=GET
      - reasonable parameters
     - BUT operationKey parameter missing (does not mean empty string)"</v>
       </c>
@@ -2872,19 +2891,19 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList")
+- Extracting authorization from config file")
 &amp;CONCATENATE("
   - POST ",G$3,"
-    - all attributes filled with chosen http-c and admin-p with method=GET
+    - all attributes filled with chosen http-c with method=GET
      - reasonable parameters
      - BUT operationKey parameter with random dummy value")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
-    - all attributes filled with chosen http-c and admin-p with method=GET
+    - all attributes filled with chosen http-c with method=GET
      - reasonable parameters
      - BUT operationKey parameter with random dummy value</v>
       </c>
@@ -3034,6 +3053,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
@@ -3181,6 +3201,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
@@ -3277,7 +3298,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="60"/>
+      <c r="A41" s="59"/>
       <c r="B41" s="8" t="s">
         <v>31</v>
       </c>
@@ -3331,6 +3352,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
@@ -3338,7 +3360,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="60"/>
+      <c r="A42" s="59"/>
       <c r="B42" s="8" t="s">
         <v>38</v>
       </c>
@@ -3384,7 +3406,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="60"/>
+      <c r="A43" s="59"/>
       <c r="B43" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3438,7 +3460,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="60"/>
+      <c r="A45" s="59"/>
       <c r="B45" s="8" t="s">
         <v>41</v>
       </c>
@@ -3459,7 +3481,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="60"/>
+      <c r="A46" s="59"/>
       <c r="B46" s="8" t="s">
         <v>42</v>
       </c>
@@ -3500,7 +3522,7 @@
 its corresponding op-c, http-c and tcp-c, storing them for later verification request
 - searching CC for op-s of ",E3,", storing operation-key")
 &amp;CONCATENATE("
-- GETting EaTL/CC (while using IP and port from above)
+- GETting EaTL/CC (while using IP, protocol and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
   - POST ",E3,"
     - all attributes filed with random values
@@ -3511,7 +3533,7 @@
 -  search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
 its corresponding op-c, http-c and tcp-c, storing them for later verification request
 - searching CC for op-s of /v1/disregard-application, storing operation-key
-- GETting EaTL/CC (while using IP and port from above)
+- GETting EaTL/CC (while using IP, protocol and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
   - POST /v1/disregard-application
     - all attributes filed with random values
@@ -3548,7 +3570,7 @@
 &amp;CONCATENATE("
 - GETting EaTL/CC (while using IP and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
-  - POST ",G3,"- all attributes filled with chosen http-c and admin-p with method=GET
+  - POST ",G3,"- all attributes filled with chosen http-c with method=GET
     -operation-key from above
     - reasonable parameters")</f>
         <v>#### Preparation:
@@ -3558,13 +3580,13 @@
 `
 - GETting EaTL/CC (while using IP and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
-  - POST /v1/approve-oam-request- all attributes filled with chosen http-c and admin-p with method=GET
+  - POST /v1/approve-oam-request- all attributes filled with chosen http-c with method=GET
     -operation-key from above
     - reasonable parameters</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="60"/>
+      <c r="A47" s="59"/>
       <c r="B47" s="8" t="s">
         <v>43</v>
       </c>
@@ -3603,14 +3625,14 @@
       <c r="E47" s="30" t="str">
         <f>CONCATENATE("#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response for entry with application-name==AA and operation-name==", E3, "
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response for entry with application-name==AA and operation-name==/v1/disregard-application
@@ -3650,7 +3672,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="60"/>
+      <c r="A48" s="59"/>
       <c r="B48" s="9" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3715,7 +3737,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A51" s="60"/>
+      <c r="A51" s="59"/>
       <c r="B51" s="12" t="s">
         <v>47</v>
       </c>
@@ -3748,14 +3770,15 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="60"/>
+    <row r="52" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="59"/>
       <c r="B52" s="13" t="s">
         <v>48</v>
       </c>
@@ -3769,14 +3792,14 @@
         <v>101</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>48</v>
+        <v>158</v>
       </c>
       <c r="G52" s="51" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="60"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="14" t="s">
         <v>49</v>
       </c>
@@ -3801,7 +3824,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="59" t="s">
+      <c r="A54" s="60" t="s">
         <v>50</v>
       </c>
       <c r="B54" s="11" t="s">
@@ -3824,7 +3847,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="59"/>
+      <c r="A55" s="60"/>
       <c r="B55" s="12" t="s">
         <v>52</v>
       </c>
@@ -3860,7 +3883,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A56" s="59"/>
+      <c r="A56" s="60"/>
       <c r="B56" s="13" t="s">
         <v>53</v>
       </c>
@@ -3881,7 +3904,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="59"/>
+      <c r="A57" s="60"/>
       <c r="B57" s="14" t="s">
         <v>49</v>
       </c>
@@ -3902,7 +3925,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="59"/>
+      <c r="A58" s="60"/>
       <c r="B58" s="13" t="s">
         <v>54</v>
       </c>
@@ -3949,7 +3972,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="232" x14ac:dyDescent="0.35">
-      <c r="A60" s="60"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="8" t="s">
         <v>57</v>
       </c>
@@ -4018,7 +4041,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
 - PUTting op-s-configuration/life-cycle-state with random alternative value")
 &amp;CONCATENATE("
   - POST ",G3,"
@@ -4029,7 +4052,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
 - PUTting op-s-configuration/life-cycle-state with random alternative value
   - POST /v1/approve-oam-request
     - all attributes filled with random values
@@ -4038,7 +4061,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A61" s="60"/>
+      <c r="A61" s="59"/>
       <c r="B61" s="8" t="s">
         <v>58</v>
       </c>
@@ -4059,7 +4082,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="60"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="15" t="s">
         <v>59</v>
       </c>
@@ -4159,7 +4182,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList")
+- Extracting authorization from config file")
 &amp;CONCATENATE("
   - POST ",G3,"
    - all attributes filled with random values
@@ -4169,7 +4192,7 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
    - all attributes filled with random values
     -operation-key from above
@@ -4236,7 +4259,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="58" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>65</v>
@@ -4313,7 +4336,7 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key- randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList")
+- Extracting authorization from config file")
 &amp;CONCATENATE("
   - POST ",G3,"
     - all attributes filled with chosen values  BUT application-release-number attribute with random dummy value differing from pattern in different ways
@@ -4322,7 +4345,7 @@
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key- randomly choosing http-c from ltpList
-- randomly choosing authorization from profileList
+- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen values  BUT application-release-number attribute with random dummy value differing from pattern in different ways
     -operation-key from above
@@ -4391,7 +4414,9 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="58"/>
+      <c r="A71" s="58" t="s">
+        <v>64</v>
+      </c>
       <c r="B71" s="7" t="s">
         <v>67</v>
       </c>
@@ -4492,7 +4517,9 @@
       <c r="G75" s="25"/>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="58"/>
+      <c r="A76" s="58" t="s">
+        <v>160</v>
+      </c>
       <c r="B76" s="7" t="s">
         <v>70</v>
       </c>
@@ -4827,7 +4854,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A96" s="59" t="s">
+      <c r="A96" s="60" t="s">
         <v>81</v>
       </c>
       <c r="B96" s="7" t="s">
@@ -4850,7 +4877,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" s="59"/>
+      <c r="A97" s="60"/>
       <c r="B97" s="8"/>
       <c r="C97" s="32" t="s">
         <v>101</v>
@@ -4866,7 +4893,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A98" s="59"/>
+      <c r="A98" s="60"/>
       <c r="B98" s="8" t="s">
         <v>41</v>
       </c>
@@ -4884,7 +4911,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="261" x14ac:dyDescent="0.35">
-      <c r="A99" s="59"/>
+      <c r="A99" s="60"/>
       <c r="B99" s="8" t="s">
         <v>83</v>
       </c>
@@ -4902,7 +4929,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A100" s="59"/>
+      <c r="A100" s="60"/>
       <c r="B100" s="8" t="s">
         <v>84</v>
       </c>
@@ -4912,7 +4939,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A101" s="59"/>
+      <c r="A101" s="60"/>
       <c r="B101" s="15" t="s">
         <v>49</v>
       </c>
@@ -4922,7 +4949,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A102" s="59"/>
+      <c r="A102" s="60"/>
       <c r="B102" s="13" t="s">
         <v>54</v>
       </c>
@@ -4932,7 +4959,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A103" s="59" t="s">
+      <c r="A103" s="60" t="s">
         <v>85</v>
       </c>
       <c r="B103" s="7" t="s">
@@ -4955,7 +4982,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A104" s="59"/>
+      <c r="A104" s="60"/>
       <c r="B104" s="8" t="s">
         <v>41</v>
       </c>
@@ -4973,7 +5000,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="59"/>
+      <c r="A105" s="60"/>
       <c r="B105" s="8" t="s">
         <v>83</v>
       </c>
@@ -4991,7 +5018,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="59"/>
+      <c r="A106" s="60"/>
       <c r="B106" s="8" t="s">
         <v>87</v>
       </c>
@@ -5001,7 +5028,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A107" s="59"/>
+      <c r="A107" s="60"/>
       <c r="B107" s="15" t="s">
         <v>49</v>
       </c>
@@ -5011,7 +5038,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A108" s="59"/>
+      <c r="A108" s="60"/>
       <c r="B108" s="13" t="s">
         <v>54</v>
       </c>
@@ -5021,7 +5048,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A109" s="59" t="s">
+      <c r="A109" s="60" t="s">
         <v>88</v>
       </c>
       <c r="B109" s="7" t="s">
@@ -5044,7 +5071,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A110" s="59"/>
+      <c r="A110" s="60"/>
       <c r="B110" s="8" t="s">
         <v>41</v>
       </c>
@@ -5062,7 +5089,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A111" s="59"/>
+      <c r="A111" s="60"/>
       <c r="B111" s="8" t="s">
         <v>83</v>
       </c>
@@ -5080,28 +5107,28 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A112" s="59"/>
+      <c r="A112" s="60"/>
       <c r="B112" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C112" s="30"/>
     </row>
     <row r="113" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A113" s="59"/>
+      <c r="A113" s="60"/>
       <c r="B113" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C113" s="30"/>
     </row>
     <row r="114" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A114" s="59"/>
+      <c r="A114" s="60"/>
       <c r="B114" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C114" s="30"/>
     </row>
     <row r="115" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A115" s="59" t="s">
+      <c r="A115" s="60" t="s">
         <v>91</v>
       </c>
       <c r="B115" s="7" t="s">
@@ -5124,7 +5151,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A116" s="59"/>
+      <c r="A116" s="60"/>
       <c r="B116" s="8" t="s">
         <v>41</v>
       </c>
@@ -5142,7 +5169,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A117" s="60"/>
+      <c r="A117" s="59"/>
       <c r="B117" s="8" t="s">
         <v>83</v>
       </c>
@@ -5160,13 +5187,13 @@
       </c>
     </row>
     <row r="118" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A118" s="60"/>
+      <c r="A118" s="59"/>
       <c r="B118" s="8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A119" s="60"/>
+      <c r="A119" s="59"/>
       <c r="B119" s="8" t="s">
         <v>49</v>
       </c>
@@ -5175,7 +5202,7 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A120" s="60"/>
+      <c r="A120" s="59"/>
       <c r="B120" s="16" t="s">
         <v>54</v>
       </c>
@@ -5184,7 +5211,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="60"/>
+      <c r="A121" s="59"/>
       <c r="C121" s="30"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -5193,6 +5220,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A115:A121"/>
     <mergeCell ref="A59:A62"/>
@@ -5202,16 +5239,6 @@
     <mergeCell ref="A76:A81"/>
     <mergeCell ref="A82:A87"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A88:A93"/>
     <mergeCell ref="A96:A102"/>
     <mergeCell ref="A103:A108"/>

</xml_diff>

<commit_message>
bequeath-your-data-and-die forwarding, updated code for the comments.
</commit_message>
<xml_diff>
--- a/testing/AA-v1+testcase.docs.xlsx
+++ b/testing/AA-v1+testcase.docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW\AdministratorAdministration\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA27C66-C91A-47FA-A8AA-78B360C58FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD4F01A-58B1-459C-8009-7367B256A4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="163">
   <si>
     <t>Testcases</t>
   </si>
@@ -467,11 +467,6 @@
     <t>/v1/list-applications</t>
   </si>
   <si>
-    <t>#### Clearing:
-- PUT NewRelease/remote-address with original value
-- PUT NewRelease/remote-port with original value</t>
-  </si>
-  <si>
     <t xml:space="preserve">## Gets the service consumption indicated to EaTL and the Parameters of the request processed?
 </t>
   </si>
@@ -481,10 +476,6 @@
   <si>
     <t>#### Clearing
 - PUT configured values with initial original values</t>
-  </si>
-  <si>
-    <t>#### Clearance check:
-- Check if the profile-collection instance is the same as initial configuration</t>
   </si>
   <si>
     <t>#### Testing:
@@ -492,59 +483,10 @@
 - checking for lifeCycleState being identical with alternative op-s-configuration/life-cycle-state</t>
   </si>
   <si>
-    <t>#### Clearing:
-- PUTting op-s-configuration/life-cycle-state back to original value
-- PUT NewRelease/remote-address with original value
-- PUT NewRelease/remote-port with original value</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/regard-application, storing operation-key
-- searching CC for op-s of /v1/disregard-application, storing operation-key
-- POST /v1/regard-application with
-  - dummy values generated for application-name, release-number
-   -operation-key from above
-   - reasonable parameter</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/regard-application, storing operation-key
-- searching CC for op-s of /v1/disregard-application, storing operation-key
-- POST /v1/regard-application with
-  - dummy values generated for application-name, release-number
-   -operation-key from above
-   - reasonable parameter
- - - GETing CC (/core-model-1-4:control-construct)
-   -Search  CC/profile-collection for entry having application-name=dummyApplicationName and release-number=dummyReleaseNumber
-   - store the instance
-- POST /v1/disregard-application with 
-    - application-name= dummyApplicationName and release-number=dummyReleaseNumber</t>
-  </si>
-  <si>
     <t>#### Testing:
 - checking for ResponseCode==204
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for http-c of NewRelease and check if the release-number is updated with dummyValue.</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- checking for ResponseCode==204
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC forapplictaion-profile of application-name=dummyApplicationName and its corresponding release-number and default value of approval-status= REGISTERED</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- checking for ResponseCode==204
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC forapplictaion-profile of application-name=dummyApplicationName and its corresponding release-number to be absent</t>
-  </si>
-  <si>
-    <t>#### Clearing:
-- PUT NewRelease/release-number with original value
-- PUT NewRelease/remote-address with original value
-- PUT NewRelease/remote-port with original value</t>
   </si>
   <si>
     <t>#### Clearing:
@@ -560,20 +502,7 @@
 - Check if the forwarding-construct instance is the same as initial configuration</t>
   </si>
   <si>
-    <t>#### Clearance check:
-- Check if the profile list is same as initial configuration</t>
-  </si>
-  <si>
     <t>BequeathingDataAndDieCausesForwardings</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response 
-   - checking same record for containing DummyXCorrelator and applicatin-name and release-number with randomly chosen values</t>
   </si>
   <si>
     <t>## Get disregard-appplication delete fc-port</t>
@@ -584,16 +513,6 @@
 - Check if the forwarding-construct is the same as initial value</t>
   </si>
   <si>
-    <t xml:space="preserve">#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response 
-   - checking same record for containing DummyXCorrelator and application-name=ApplicationLaterTopology, operation-name=/v1/update-ltp, trace-indicator=expected unique trace-indicator(values appened with unique numbers) and other attributes as expected.
-</t>
-  </si>
-  <si>
     <t>##Gets new-application-address update trigger update-ltp to ALT?</t>
   </si>
   <si>
@@ -603,23 +522,7 @@
     <t>##Gets disregard-application trigger delete-ltp-and-dependents to ALT?</t>
   </si>
   <si>
-    <t xml:space="preserve">#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response 
-   - checking same record for containing DummyXCorrelator and application-name=ApplicationLaterTopology, operation-name=/v1/update-fc, trace-indicator=expected unique trace-indicator(values appened with unique numbers) and other attributes as expected.
-</t>
-  </si>
-  <si>
     <t>NewApplicationCausesRequestForInquiringOamRequestApprovals</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- checking for ResponseCode==204
-- GETing CC (/core-model-1-4:control-construct)
-- search for operation-client uuid of redirect-service-request-information of the random application. Find the fc OUTPUT-port list of NewApplicationCausesRequestForInquiringOamRequestApprovals with logical-termination-point having value as the dummy etracted op-c of  redirect-service-request-information</t>
   </si>
   <si>
     <t xml:space="preserve">#### Testing:
@@ -629,30 +532,6 @@
 </t>
   </si>
   <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/regard-application, storing operation-key
-- searching CC for op-s of /v1/disregard-application, storing operation-key
-- POST /v1/regard-application with
-  - dummy values generated for application-name, release-number
-   -operation-key from above
-   - reasonable parameter
-- GET control-construct, search for operation-client redirect-service-request-information under the newly created application, store the operation-key
- Find the fc OUTPUT-port list of NewApplicationCausesRequestForInquiringOamRequestApprovals with logical-termination-point having value as the dummy etracted op-c of  redirect-service-request-information
-- POST /v1/disregard-application
-     - with attributes filled with random values
-     - operation-key from above</t>
-  </si>
-  <si>
-    <t>#### Testing:
-- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
-   - operation-key from above
-   - DummyValue of x-correlator
-   - checking response 
-   - checking same record for containing DummyXCorrelator and application-name=ApplicationLaterTopology, operation-name=/v1/delete-ltp-and-dependents, trace-indicator=expected unique trace-indicator(values appened with unique numbers) and other attributes as expected.</t>
-  </si>
-  <si>
     <t>/v1/approve-oam-request</t>
   </si>
   <si>
@@ -681,85 +560,6 @@
   </si>
   <si>
     <t>AdministratorAdministration</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
-- POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
-   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
-   -operation-key from above
-   - reasonable parameter</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
-- POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
-   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
-    -operation-key from above
-    - all parameters with realistic values, BUT 
-          1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
-- POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
-   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
-    -operation-key from above
-     - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string).</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
-- POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
-   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
-    -operation-key from above
-   - all parameters with realistic values, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
-- POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
-   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
-    - all parameters with reasonable values
-   - BUT operationKey parameter missing (does not mean empty string)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
-- POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
-   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!) 
-    - all parameters with reasonable values
-   - BUT operationKey parameter with random dummy value.
-</t>
   </si>
   <si>
     <t>#### Preparation:
@@ -785,31 +585,136 @@
    - all parameters with realistic values (incl. DummyXCorrelator)</t>
   </si>
   <si>
+    <t>#### Clearing:
+- PUT NewRelease/release-number with original value
+- PUT NewRelease/remote-address with original value
+- PUT NewRelease/remote-protocol with original value
+- PUT NewRelease/remote-port with original value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### Testing:
+- Checking for response-code 200
+- Extract applicationName, releaseNumber, address, protocol and port from output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals and store it in expectedApplicationsList.
+- Generate schema based on the specification
+- Checking the response body for each attribute against the generated schema
+- Checking the response body attributes against expectedApplicationsList.
+</t>
+  </si>
+  <si>
+    <t>Request body Attribute correctness?</t>
+  </si>
+  <si>
+    <t>Forwardings triggered?</t>
+  </si>
+  <si>
     <t>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
 - searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
 - POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
+   - new-application-name and new-application-release according to chosen http-c
+   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
+   -operation-key from above
+   - reasonable parameter</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
+- POST /v1/bequeath-your-data-and-die with
+   - new-application-name and new-application-release according to chosen http-c
    - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
    -operation-key from above
    - all parameters with realistic values, BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)</t>
   </si>
   <si>
+    <t>#### Clearing:
+- PUT NewRelease/remote-protocol with original value
+- PUT NewRelease/remote-address with original value
+- PUT NewRelease/remote-port with original value</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- PUTting op-s-configuration/life-cycle-state back to original value
+- PUT NewRelease/remote-protocol with original value
+- PUT NewRelease/remote-address with original value
+- PUT NewRelease/remote-port with original value</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- PUT NewRelease/release-number with original value
+- PUT NewRelease/remote-protocol with original value
+- PUT NewRelease/remote-address with original value
+- PUT NewRelease/remote-port with original value</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
+- POST /v1/bequeath-your-data-and-die with
+   - new-application-name and new-application-release according to chosen http-c
+   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
+    -operation-key from above
+    - all parameters with realistic values, BUT 
+          1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
+- POST /v1/bequeath-your-data-and-die with
+   - new-application-name and new-application-release according to chosen http-c
+   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
+    -operation-key from above
+     - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string).</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
+- POST /v1/bequeath-your-data-and-die with
+   - new-application-name and new-application-release according to chosen http-c
+   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
+    -operation-key from above
+   - all parameters with realistic values, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
+- POST /v1/bequeath-your-data-and-die with
+   - new-application-name and new-application-release according to chosen http-c
+   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
+    - all parameters with reasonable values
+   - BUT operationKey parameter missing (does not mean empty string)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
+- POST /v1/bequeath-your-data-and-die with
+   - new-application-name and new-application-release according to chosen http-c
+   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!) 
+    - all parameters with reasonable values
+   - BUT operationKey parameter with random dummy value.
+</t>
+  </si>
+  <si>
     <t>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
    - search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
 its corresponding op-c, http-c and tcp-c, storing them for later verification request.
 - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
 - searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
-- GETting EaTL/CC (while using IP and port from above)
+- GETting EaTL/CC (while using IP, protocol and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
 - POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
+   - new-application-name and new-application-release according to chosen http-c
    - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!) 
    -operation-key from above
    - all parameters with realistic values (incl. DummyXCorrelator)")</t>
@@ -818,12 +723,10 @@
     <t>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
 - searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them.
 - PUTting op-s-configuration/life-cycle-state with random alternative value
 - POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
+   - new-application-name and new-application-release according to chosen http-c
    - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
    -operation-key from above
    - reasonable parameter</t>
@@ -832,11 +735,9 @@
     <t xml:space="preserve">#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
 - searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them.
  POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
+   - new-application-name and new-application-release according to chosen http-c
    - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!), BUT one randomly chosen attribute missing
     -operation-key from above
     - reasonable parameters
@@ -845,9 +746,144 @@
   <si>
     <t>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
+- search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
+its corresponding op-c, http-c and tcp-c, storing them for later verification request 
+- searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them.
+- GETting EaTL/CC (while using IP, protocol and port from above)
+   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
+ POST /v1/bequeath-your-data-and-die with
+   - new-application-name and new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!), BUT new-application-release attribute with random dummy value that matches the specified pattern.
+    -operation-key from above
+    - reasonable parameters</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response 
+   - checking same record for containing DummyXCorrelator and other attributes with randomly chosen values.</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+   -  search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
+its corresponding op-c, http-c and tcp-c, storing them for later verification request
+   - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
+  - find http-s and tcp-s from CC, store them
+   - searcing CC for output port of PromptForEmbeddingCausesRequestForBequeathingData (fc related with OldRelease), find corresponding op-c, http-c and tcp-c, store them
+- GETing CC (/core-model-1-4:control-construct) with OldRelase
+  - getting required attributes and store them.
+- GETting EaTL/CC (while using IP and port from above)
+   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
+- POST /v1/bequeath-your-data-and-die with  
+     - Request body attributes according to chosen http-s, tcp-s (i.e NewRelease)
+     - Request URL attributes according to chosen http-c and tcp-c of Old Release
+     - operation-key from above
+   - all parameters with realistic values (incl. DummyXCorrelator)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response 
+   - checking same record for containing DummyXCorrelator and application-name=ApplicationLayerTopology, operation-name=/v1/update-ltp, trace-indicator=expected unique trace-indicator(values appened with unique numbers) and other attributes as expected.
+</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
+ POST /v1/bequeath-your-data-and-die with
+ - new-application-name and new-application-release according to chosen http-c  
+ - new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!), BUT one randomly chosen attribute missing
+    -operation-key from above
+    - reasonable parameters</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
+- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
+ POST /v1/bequeath-your-data-and-die with
+   - new-application-name and new-application-release according to chosen http-c
+   - new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!), BUT new-application-name attribute with random dummy value.
+    -operation-key from above
+    - reasonable parameters</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/regard-application, storing operation-key
+- searching CC for op-s of /v1/disregard-application, storing operation-key
+- POST /v1/regard-application with
+  - with all attributes according to values chosen from above, BUT the chosen attribute with random dummy value (that matches the specified pattern in OAS)
+   -operation-key from above
+   - reasonable parameter</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response 
+   - checking same record for containing DummyXCorrelator and applicatin-name and release-number with randomly chosen values</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- checking for ResponseCode==204
+- GETing CC (/core-model-1-4:control-construct)
+- search for operation-client uuid of redirect-service-request-information of the random application. Find the fc OUTPUT-port list of NewApplicationCausesRequestForInquiringOamRequestApprovals with logical-termination-point having value as the dummy extracted op-c of  redirect-service-request-information</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/regard-application, storing operation-key
+- searching CC for op-s of /v1/disregard-application, storing operation-key
+- searching CC for output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals, find corresponding operation client and store them.
+- POST /v1/regard-application with
+  - dummy values generated for application-name, release-number
+   -operation-key from above
+   - reasonable parameter</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
 -  search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
 its corresponding op-c, http-c and tcp-c, storing them for later verification request. 
-- also searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
+- searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
+- searching CC for op-s of /v1/regard-application, storing operation-key
+- searching CC for output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals, find corresponding operation client and store them.
+- GETting EaTL/CC (while using IP and port from above)
+   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
+- POST /v1/regard-application with
+  - dummy values generated for application-name, release-number, address, port 
+   -operation-key from above
+   - reasonable parameter</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- /v1/disregard-application with values according to generated dummy values.
+-  any attributes are used with dummy values then revert with intial value.</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- /v1/disregard-application with values according to generated dummy values.
+-  any attributes are used with dummy values then revert with intial value</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+-  search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
+its corresponding op-c, http-c and tcp-c, storing them for later verification request 
+- searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
 - searching CC for op-s of /v1/regard-application, storing operation-key
 - GETting EaTL/CC (while using IP and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
@@ -857,14 +893,59 @@
    - reasonable parameter</t>
   </si>
   <si>
+    <t xml:space="preserve">#### Testing:
+- POST ExecutionAndTraceLog/v1/list-records-of-flow with 
+   - IP, protocol and port from above
+   - operation-key from above
+   - DummyValue of x-correlator
+   - checking response 
+   - checking same record for containing DummyXCorrelator and application-name=ApplicationLayerTopology, operation-name=/v1/update-fc, trace-indicator=expected unique trace-indicator(values appened with unique numbers) and other attributes as expected.
+</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/regard-application, storing operation-key
+- searching CC for op-s of /v1/disregard-application, storing operation-key
+- POST /v1/regard-application with
+  - dummy values generated for application-name, release-number
+   -operation-key from above
+   - reasonable parameter
+ - - GETing CC (/core-model-1-4:control-construct)
+   -Search  CC/httpClientLtp with application-name=dummyApplicationName and release-number=dummyReleaseNumber and store the httpClientLtp
+- POST /v1/disregard-application with 
+    - application-name= dummyApplicationName and release-number=dummyReleaseNumber</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- checking for ResponseCode==204
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC/httpClientLtp of application-name=dummyApplicationName and its corresponding release-number to be absent</t>
+  </si>
+  <si>
+    <t>#### Preparation:
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC for op-s of /v1/regard-application, storing operation-key
+- searching CC for op-s of /v1/disregard-application, storing operation-key
+- POST /v1/regard-application with
+  - dummy values generated for application-name, release-number, protocol, address, port
+   -operation-key from above
+   - reasonable parameter
+- GET control-construct, search for operation-client redirect-service-request-information under the newly created application, store the operation-key
+ Find the fc OUTPUT-port list of NewApplicationCausesRequestForInquiringOamRequestApprovals with logical-termination-point having value as the dummy etracted op-c of  redirect-service-request-information
+- POST /v1/disregard-application
+     - with attributes filled with random values
+     - operation-key from above</t>
+  </si>
+  <si>
     <t>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)   
 -  search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
 its corresponding op-c, http-c and tcp-c, storing them for later verification request.
-- also searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
+- searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
 - searching CC for op-s of /v1/regard-application, storing operation-key
 - POST /v1/regard-application with
-  - dummy values generated for application-name, release-number, address, port
+  - dummy values generated for application-name, release-number, address, protocol, port
    -operation-key from above
    - reasonable parameter
 - search CC for created http-c, tcp-c , search for the logical-termination-point=op-c of inquire-oam-request-approval  in OUTPUT port of FC=NewApplicationCausesRequestForInquiringOamRequestApprovals, store the local-id
@@ -873,113 +954,30 @@
    - all parameters with random DummyValues</t>
   </si>
   <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
--  search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
-its corresponding op-c, http-c and tcp-c, storing them for later verification request 
-- also searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
-- searching CC for op-s of /v1/regard-application, storing operation-key
-- GETting EaTL/CC (while using IP and port from above)
-   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
-- POST /v1/regard-application with
-  - dummy values generated for application-name, release-number, address, port 
-   -operation-key from above
-   - reasonable parameter</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
-its corresponding op-c, http-c and tcp-c, storing them for later verification request 
-- also searching CC for output-fc-port of ServiceRequestCausesLtpUpdateRequest, its corresponding op-c, http-c, storing them.
-- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them.
-- GETting EaTL/CC (while using IP and port from above)
-   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
- POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to http-s
-   - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!), BUT new-application-release attribute with random dummy value that matches the specified pattern.
-    -operation-key from above
-    - reasonable parameters</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
- POST /v1/bequeath-your-data-and-die with
-   - with all attributes according to values chosen from above, BUT the chosen attribute with random dummy value (that does not comply specification).
-    -operation-key from above
-    - reasonable parameters</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
-- searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
- POST /v1/bequeath-your-data-and-die with
-   - with all attributes according to values chosen from above, BUT the chosen attribute with random dummy value (that does not comply specification)
-    -operation-key from above
-    - reasonable parameters</t>
-  </si>
-  <si>
     <t>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response 
-   - checking same record for containing DummyXCorrelator and other attributes with randomly chosen values.</t>
-  </si>
-  <si>
-    <t>#### Clearing:
-- PUT NewRelease/release-number with original value
-- PUT NewRelease/remote-address with original value
-- PUT NewRelease/remote-protocol with original value
-- PUT NewRelease/remote-port with original value</t>
-  </si>
-  <si>
-    <t>#### Preparation:
-- GETing CC (/core-model-1-4:control-construct)
-   -  search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
-its corresponding op-c, http-c and tcp-c, storing them for later verification request
-   - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-  - find http-s from CC, store them
-   - - searcing CC for output port of PromptForEmbeddingCausesRequestForBequeathingData (related with OldRelease), find corresponding op-c, http-c and tcp-c, store them
-- GETing CC (/core-model-1-4:control-construct) with OldRelase
-  - getting required attributes and store them.
-- GETting EaTL/CC (while using IP and port from above)
-   - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
-- POST /v1/bequeath-your-data-and-die with  
-     - application-name according to chosen http-s
-     - other attributes according to chosen http-c
-     - operation-key from above
-   - all parameters with realistic values (incl. DummyXCorrelator)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#### Testing:
-- Checking for response-code 200
-- Extract applicationName, releaseNumber, address, protocol and port from output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals and store it in expectedApplicationsList.
-- Generate schema based on the specification
-- Checking the response body for each attribute against the generated schema
-- Checking the response body attributes against expectedApplicationsList.
-</t>
-  </si>
-  <si>
-    <t>Request body Attribute correctness?</t>
-  </si>
-  <si>
-    <t>Forwardings triggered?</t>
+   - checking same record for containing DummyXCorrelator and application-name=ApplicationLayerTopology, operation-name=/v1/delete-ltp-and-dependents, trace-indicator=expected unique trace-indicator(values appened with unique numbers) and other attributes as expected.</t>
+  </si>
+  <si>
+    <t>#### Clearance check:
+- Check if the logical-temination-point instance is the same as initial configuration</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- checking for ResponseCode==204
+- GETing CC (/core-model-1-4:control-construct)
+- searching CC application-name=dummyApplicationName and its corresponding release-number updated with dummyValue.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1055,6 +1053,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1106,7 +1111,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1218,13 +1223,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1378,9 +1398,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1391,22 +1408,26 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1725,18 +1746,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6438CD8-A3F3-4ED1-9D84-D5D573F05C15}">
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D68" sqref="D68"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="57" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" style="55" customWidth="1"/>
     <col min="2" max="2" width="70.7265625" style="17"/>
     <col min="3" max="6" width="70.7265625"/>
     <col min="7" max="7" width="70.7265625" customWidth="1"/>
@@ -1744,8 +1765,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
-        <v>136</v>
+      <c r="A1" s="52" t="s">
+        <v>121</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="18"/>
@@ -1755,7 +1776,7 @@
       <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
@@ -1768,7 +1789,7 @@
       <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1787,11 +1808,11 @@
         <v>98</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="59" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1818,13 +1839,13 @@
         <v>## Is service idempotent?</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="58"/>
+    <row r="5" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="59"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D5" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -1883,26 +1904,26 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
 ")
 &amp;CONCATENATE("
   - POST ",G3,"
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
-    - reasonable parameters")</f>
+   - provide authorization from config file
+   - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
-    - reasonable parameters</v>
+   - provide authorization from config file
+   - reasonable parameters</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="58"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1935,13 +1956,13 @@
 - checking for ResponseCode==200</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="58"/>
+    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="59"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D7" s="24" t="str">
         <f>$B7</f>
@@ -1965,7 +1986,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="59" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1992,19 +2013,19 @@
         <v>## Get parameters checked for completeness?</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="58"/>
+    <row r="9" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="59"/>
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D9" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",D$3,", storing operation-key
--  searching CC for output fc-port of E9, find corresponding op-c, http-c and tcp-c, store them")
+-  searching CC for output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals, find corresponding op-c, http-c and tcp-c, store them")
 &amp;CONCATENATE("
   - POST ",D$3,"
      - all attributes according to chosen http-c, tcp-c
@@ -2013,7 +2034,7 @@
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/regard-application, storing operation-key
--  searching CC for output fc-port of E9, find corresponding op-c, http-c and tcp-c, store them
+-  searching CC for output fc-port of NewApplicationCausesRequestForInquiringOamRequestApprovals, find corresponding op-c, http-c and tcp-c, store them
   - POST /v1/regard-application
      - all attributes according to chosen http-c, tcp-c
     -operation-key from above
@@ -2055,26 +2076,26 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key
-- randomly choosing http-c from ltpList
-- Extracting authorization from config file")
+- randomly choosing http-c from ltpList")
 &amp;CONCATENATE("
  - POST ",G3,"
    - all attributes filled with chosen http-c with method=GET
-    -operation-key from above
+    -operation-key from above, 
+    -authorization
     -  BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
  - POST /v1/approve-oam-request
    - all attributes filled with chosen http-c with method=GET
-    -operation-key from above
+    -operation-key from above, 
+    -authorization
     -  BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="58"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
@@ -2104,15 +2125,15 @@
 - checking for ResponseCode == 400</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="58"/>
+    <row r="11" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="59"/>
       <c r="B11" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D11" s="27" t="str">
         <f>$B7</f>
@@ -2136,7 +2157,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="59" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2163,13 +2184,13 @@
         <v>## Gets originator checked for compliance with specification?</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="232" x14ac:dyDescent="0.35">
-      <c r="A13" s="61"/>
+    <row r="13" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A13" s="60"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D13" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2226,26 +2247,26 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
-- randomly choosing http-c from ltpList
-- Extracting authorization from config file")
+- randomly choosing http-c from ltpList")
 &amp;CONCATENATE("
   - POST ",G$3,"
     - all attributes filled with chosen http-c with method=GET
+   - operation-key and provide authorization
      - all parameters with realistic values, BUT 
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
+   - operation-key and provide authorization
      - all parameters with realistic values, BUT 
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="61"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
@@ -2275,15 +2296,15 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="61"/>
+    <row r="15" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="60"/>
       <c r="B15" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D15" s="24" t="str">
         <f>$B7</f>
@@ -2307,7 +2328,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="59" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -2334,13 +2355,13 @@
         <v>## Gets x-correlator checked for complying the pattern?</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="232" x14ac:dyDescent="0.35">
-      <c r="A17" s="58"/>
+    <row r="17" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A17" s="59"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D17" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2397,26 +2418,26 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
-- randomly choosing http-c from ltpList
-- Extracting authorization from config file")
+- randomly choosing http-c from ltpList")
 &amp;CONCATENATE("
   - POST ",G$3,"
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
+   - provide authorization from config file
    - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
+   - provide authorization from config file
    - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="58"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
@@ -2446,15 +2467,15 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="58"/>
+    <row r="19" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A19" s="59"/>
       <c r="B19" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D19" s="31" t="str">
         <f>$B7</f>
@@ -2478,7 +2499,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="59" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -2505,13 +2526,13 @@
         <v>## Gets trace-indicator checked for complying the pattern?</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="232" x14ac:dyDescent="0.35">
-      <c r="A21" s="58"/>
+    <row r="21" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A21" s="59"/>
       <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D21" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2568,26 +2589,26 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
-- randomly choosing http-c from ltpList
-- Extracting authorization from config file")
+- randomly choosing http-c from ltpList")
 &amp;CONCATENATE("
   - POST ",G$3,"
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
+   - provide authorization from config file
    - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
+   - provide authorization from config file
    - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="58"/>
+      <c r="A22" s="59"/>
       <c r="B22" s="8" t="s">
         <v>15</v>
       </c>
@@ -2617,15 +2638,15 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="58"/>
+    <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A23" s="59"/>
       <c r="B23" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D23" s="31" t="str">
         <f>$B7</f>
@@ -2649,7 +2670,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="59" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -2676,13 +2697,13 @@
         <v>## Gets security key checked for availability?</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="58"/>
+    <row r="25" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="59"/>
       <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D25" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2729,26 +2750,26 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
-- randomly choosing http-c from ltpList
-- Extracting authorization from config file")
+- randomly choosing http-c from ltpList")
 &amp;CONCATENATE("
   - POST ",G$3,"
      - all attributes filled with chosen http-c with method=GET
+    -provide authorization from config file
      - reasonable parameters
     - BUT operationKey parameter missing (does not mean empty string)""")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
      - all attributes filled with chosen http-c with method=GET
+    -provide authorization from config file
      - reasonable parameters
     - BUT operationKey parameter missing (does not mean empty string)"</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="58"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="8" t="s">
         <v>25</v>
       </c>
@@ -2778,15 +2799,15 @@
 - checking for ResponseCode==401</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="58"/>
+    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A27" s="59"/>
       <c r="B27" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D27" s="24" t="str">
         <f>$B7</f>
@@ -2810,7 +2831,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -2837,13 +2858,13 @@
         <v>## Gets security key checked for correctness?</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="58"/>
+    <row r="29" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="59"/>
       <c r="B29" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D29" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2890,26 +2911,26 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G$3,", storing operation-key
-- randomly choosing http-c from ltpList
-- Extracting authorization from config file")
+- randomly choosing http-c from ltpList")
 &amp;CONCATENATE("
   - POST ",G$3,"
     - all attributes filled with chosen http-c with method=GET
+    - provide authorization from config file
      - reasonable parameters
      - BUT operationKey parameter with random dummy value")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
+    - provide authorization from config file
      - reasonable parameters
      - BUT operationKey parameter with random dummy value</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="58"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
       </c>
@@ -2939,15 +2960,15 @@
 - checking for ResponseCode==401</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="58"/>
+    <row r="31" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A31" s="59"/>
       <c r="B31" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D31" s="24" t="str">
         <f>$B7</f>
@@ -2971,7 +2992,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="59" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -2998,8 +3019,8 @@
         <v>## Contains response complete set of headers?</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
+    <row r="33" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="59"/>
       <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
@@ -3008,11 +3029,9 @@
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
 - searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
 - POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
+   - new-application-name and new-application-release according to chosen http-c
    - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
    -operation-key from above
    - reasonable parameter</v>
@@ -3053,20 +3072,20 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
-    - reasonable parameters</v>
+   - provide authorization from config file
+   - reasonable parameters</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A34" s="58"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D34" s="30" t="str">
         <f>$C34</f>
@@ -3081,21 +3100,21 @@
 - checking for ResponseHeaders (x-correlator, exec-time, backend-time and life-cycle-state) being present and checking for correctness of type of each parameter.</v>
       </c>
       <c r="F34" s="50" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="G34" s="50" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="58"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A35" s="59"/>
       <c r="B35" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D35" s="31" t="str">
         <f>$B7</f>
@@ -3119,7 +3138,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -3146,8 +3165,8 @@
         <v>## Is the initial x-correlator ín the response?</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="58"/>
+    <row r="37" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="59"/>
       <c r="B37" s="8" t="s">
         <v>31</v>
       </c>
@@ -3156,11 +3175,9 @@
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
 - searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
 - POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
+   - new-application-name and new-application-release according to chosen http-c
    - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
    -operation-key from above
    - reasonable parameter</v>
@@ -3201,15 +3218,15 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
-    - reasonable parameters</v>
+   - provide authorization from config file
+   - reasonable parameters</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="58"/>
+      <c r="A38" s="59"/>
       <c r="B38" s="8" t="s">
         <v>35</v>
       </c>
@@ -3232,21 +3249,21 @@
 - checking for response headers containing x-correlator==dummyXCorrelator</v>
       </c>
       <c r="F38" s="50" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="G38" s="50" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="58"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A39" s="59"/>
       <c r="B39" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D39" s="24" t="str">
         <f>$B7</f>
@@ -3270,7 +3287,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="58" t="s">
+      <c r="A40" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -3297,8 +3314,8 @@
         <v>## Is the correct life-cycle-state ín the response?</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="59"/>
+    <row r="41" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="61"/>
       <c r="B41" s="8" t="s">
         <v>31</v>
       </c>
@@ -3307,11 +3324,9 @@
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/bequeath-your-data-and-die, storing operation-key
-- find http-s from CC
 - searcing CC for output port of PromptForBequeathingDataCausesTransferOfListOfApplications, find corresponding op-c, http-c and tcp-c, store them
 - POST /v1/bequeath-your-data-and-die with
-   - new-application-name according to chosen http-s
-   - new-application-release according to chosen http-c
+   - new-application-name and new-application-release according to chosen http-c
    - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
    -operation-key from above
    - reasonable parameter</v>
@@ -3352,15 +3367,15 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
-    - reasonable parameters</v>
+   - provide authorization from config file
+   - reasonable parameters</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="59"/>
+      <c r="A42" s="61"/>
       <c r="B42" s="8" t="s">
         <v>38</v>
       </c>
@@ -3405,15 +3420,15 @@
 - checking for response headers containing life-cycle-state is equal to the value as present in the control-construct for /v1/approve-oam-request/configuration/life-cycle-state</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="59"/>
+    <row r="43" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A43" s="61"/>
       <c r="B43" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D43" s="24" t="str">
         <f>$B7</f>
@@ -3437,30 +3452,30 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="58" t="s">
+      <c r="A44" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G44" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="59"/>
+      <c r="A45" s="61"/>
       <c r="B45" s="8" t="s">
         <v>41</v>
       </c>
@@ -3480,13 +3495,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="59"/>
+    <row r="46" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="61"/>
       <c r="B46" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D46" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3522,6 +3537,7 @@
 its corresponding op-c, http-c and tcp-c, storing them for later verification request
 - searching CC for op-s of ",E3,", storing operation-key")
 &amp;CONCATENATE("
+- search CC for http-s
 - GETting EaTL/CC (while using IP, protocol and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
   - POST ",E3,"
@@ -3533,6 +3549,7 @@
 -  search CC for output fc-port of ServiceRequestCausesLoggingRequest, 
 its corresponding op-c, http-c and tcp-c, storing them for later verification request
 - searching CC for op-s of /v1/disregard-application, storing operation-key
+- search CC for http-s
 - GETting EaTL/CC (while using IP, protocol and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
   - POST /v1/disregard-application
@@ -3565,6 +3582,7 @@
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for http-c of ExecutionAndTraceLog its corresponding tcp-c and op-c of record-service-request, store them
+- find randon http-c and store
 - searching CC for op-s of ",G3,", storing operation-key
 `")
 &amp;CONCATENATE("
@@ -3572,35 +3590,38 @@
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
   - POST ",G3,"- all attributes filled with chosen http-c with method=GET
     -operation-key from above
+    - provide authorization from config file
     - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for http-c of ExecutionAndTraceLog its corresponding tcp-c and op-c of record-service-request, store them
+- find randon http-c and store
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 `
 - GETting EaTL/CC (while using IP and port from above)
    - searching CC for op-c of /v1/list-records-of-flow, storing operation-key
   - POST /v1/approve-oam-request- all attributes filled with chosen http-c with method=GET
     -operation-key from above
+    - provide authorization from config file
     - reasonable parameters</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="59"/>
+      <c r="A47" s="61"/>
       <c r="B47" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C47" s="30" t="str">
         <f>CONCATENATE("#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response for entry with application-name==AA and operation-name==", C3, "
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response for entry with application-name==AA and operation-name==/v1/bequeath-your-data-and-die
@@ -3641,14 +3662,14 @@
       <c r="F47" s="30" t="str">
         <f>CONCATENATE("#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response for entry with application-name==AA and operation-name==", F3, "
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response for entry with application-name==AA and operation-name==/v1/list-applications
@@ -3657,29 +3678,29 @@
       <c r="G47" s="30" t="str">
         <f>CONCATENATE("#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response for entry with application-name==AA and operation-name==", G3, "
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator")</f>
         <v>#### Testing:
 - POST ExecutionAndTraceLog/v1/list-records-of-flow with 
-   - IP and port from above
+   - IP, protocol and port from above
    - operation-key from above
    - DummyValue of x-correlator
    - checking response for entry with application-name==AA and operation-name==/v1/approve-oam-request
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="59"/>
+    <row r="48" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="61"/>
       <c r="B48" s="9" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D48" s="33" t="str">
         <f>$B7</f>
@@ -3703,7 +3724,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="54" t="s">
         <v>44</v>
       </c>
       <c r="B49" s="10"/>
@@ -3714,7 +3735,7 @@
       <c r="G49" s="35"/>
     </row>
     <row r="50" spans="1:7" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="59" t="s">
         <v>45</v>
       </c>
       <c r="B50" s="11" t="s">
@@ -3733,22 +3754,22 @@
         <v>46</v>
       </c>
       <c r="G50" s="36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A51" s="59"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="61"/>
       <c r="B51" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F51" s="37" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -3770,47 +3791,47 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen http-c with method=GET
     -operation-key from above
-    - reasonable parameters</v>
+   - provide authorization from config file
+   - reasonable parameters</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="59"/>
+      <c r="A52" s="61"/>
       <c r="B52" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="G52" s="51" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="59"/>
+      <c r="A53" s="61"/>
       <c r="B53" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C53" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F53" s="39" t="str">
         <f>$B7</f>
@@ -3824,7 +3845,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="60" t="s">
+      <c r="A54" s="62" t="s">
         <v>50</v>
       </c>
       <c r="B54" s="11" t="s">
@@ -3846,105 +3867,111 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="60"/>
+    <row r="55" spans="1:7" ht="174" x14ac:dyDescent="0.35">
+      <c r="A55" s="62"/>
       <c r="B55" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F55" s="37" t="str">
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct
      - searching CC for op-s of ",F3,", storing it.
-     - search for random  application-p, store it
-     - PUT random values to each configurable parameters of chosen application-p, store dummy values
+- POST ",F3," with
+   - operation-key from above
+   - reasonable parameters 
+   - response: extract random httpc-c
+- PUT random values to each configurable parameters of chosen http-c, store dummy values
 - POST ",F3," with
       - operation-key from above
       - reasonable parameters ")</f>
         <v xml:space="preserve">#### Preparation:
 - GETing CC (/core-model-1-4:control-construct
      - searching CC for op-s of /v1/list-applications, storing it.
-     - search for random  application-p, store it
-     - PUT random values to each configurable parameters of chosen application-p, store dummy values
+- POST /v1/list-applications with
+   - operation-key from above
+   - reasonable parameters 
+   - response: extract random httpc-c
+- PUT random values to each configurable parameters of chosen http-c, store dummy values
 - POST /v1/list-applications with
       - operation-key from above
       - reasonable parameters </v>
       </c>
       <c r="G55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A56" s="60"/>
+      <c r="A56" s="62"/>
       <c r="B56" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F56" s="25" t="s">
         <v>53</v>
       </c>
       <c r="G56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="60"/>
+      <c r="A57" s="62"/>
       <c r="B57" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C57" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="D57" t="s">
-        <v>101</v>
-      </c>
-      <c r="E57" t="s">
-        <v>101</v>
-      </c>
-      <c r="F57" s="39" t="s">
-        <v>102</v>
-      </c>
       <c r="G57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="60"/>
+      <c r="A58" s="62"/>
       <c r="B58" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C58" s="25"/>
       <c r="D58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="G58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="58" t="s">
+      <c r="A59" s="59" t="s">
         <v>55</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -3971,13 +3998,13 @@
         <v>## Gets lifeCycleState propagated?</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="232" x14ac:dyDescent="0.35">
-      <c r="A60" s="59"/>
+    <row r="60" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A60" s="61"/>
       <c r="B60" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D60" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4041,27 +4068,27 @@
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
 - PUTting op-s-configuration/life-cycle-state with random alternative value")
 &amp;CONCATENATE("
   - POST ",G3,"
     - all attributes filled with random values
     -operation-key from above
+   - provide authorization from config file
     - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
 - PUTting op-s-configuration/life-cycle-state with random alternative value
   - POST /v1/approve-oam-request
     - all attributes filled with random values
     -operation-key from above
+   - provide authorization from config file
     - reasonable parameters</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A61" s="59"/>
+      <c r="A61" s="61"/>
       <c r="B61" s="8" t="s">
         <v>58</v>
       </c>
@@ -4075,19 +4102,19 @@
         <v>58</v>
       </c>
       <c r="F61" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G61" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="59"/>
+    <row r="62" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="61"/>
       <c r="B62" s="15" t="s">
         <v>59</v>
       </c>
       <c r="C62" s="40" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="D62" s="40" t="s">
         <v>59</v>
@@ -4103,7 +4130,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="58" t="s">
+      <c r="A63" s="59" t="s">
         <v>60</v>
       </c>
       <c r="B63" s="7" t="s">
@@ -4130,13 +4157,13 @@
         <v>## Get attributes checked for completeness?</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="232" x14ac:dyDescent="0.35">
-      <c r="A64" s="58"/>
+    <row r="64" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A64" s="59"/>
       <c r="B64" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D64" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4175,32 +4202,32 @@
     - reasonable parameters</v>
       </c>
       <c r="F64" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G64" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of ",G3,", storing operation-key
-- randomly choosing http-c from ltpList
-- Extracting authorization from config file")
+- randomly choosing http-c from ltpList")
 &amp;CONCATENATE("
   - POST ",G3,"
    - all attributes filled with random values
     -operation-key from above
+    - provide authorization from config file
     - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key
 - randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
    - all attributes filled with random values
     -operation-key from above
+    - provide authorization from config file
     - reasonable parameters</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="58"/>
+      <c r="A65" s="59"/>
       <c r="B65" s="8" t="s">
         <v>63</v>
       </c>
@@ -4220,7 +4247,7 @@
 - checking for ResponseCode==400</v>
       </c>
       <c r="F65" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G65" s="26" t="str">
         <f ca="1">$C65</f>
@@ -4229,7 +4256,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="58"/>
+      <c r="A66" s="59"/>
       <c r="B66" s="15" t="s">
         <v>49</v>
       </c>
@@ -4249,7 +4276,7 @@
 - not applicable</v>
       </c>
       <c r="F66" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G66" s="24" t="str">
         <f>$B7</f>
@@ -4258,8 +4285,8 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="58" t="s">
-        <v>159</v>
+      <c r="A67" s="59" t="s">
+        <v>126</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>65</v>
@@ -4285,13 +4312,13 @@
         <v>## Get each attributes checked for correctness?</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="174" x14ac:dyDescent="0.35">
-      <c r="A68" s="58"/>
+    <row r="68" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="59"/>
       <c r="B68" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D68" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -4300,7 +4327,7 @@
 - searching CC for an instance of already existing random http-c and its corresponding tcp-c, store them")
 &amp;CONCATENATE("
   - POST ",D3,"
-    - all attributes according to chosen http-c and tcp-c  BUT application-name attribute with random dummy value with length&lt;3
+    - with all attributes according to values chosen from above, BUT the chosen attribute with random dummy value (that does not comply specification)
     -operation-key from above
     - reasonable parameters")</f>
         <v>#### Preparation:
@@ -4308,7 +4335,7 @@
 - searching CC for op-s of /v1/regard-application, storing operation-key
 - searching CC for an instance of already existing random http-c and its corresponding tcp-c, store them
   - POST /v1/regard-application
-    - all attributes according to chosen http-c and tcp-c  BUT application-name attribute with random dummy value with length&lt;3
+    - with all attributes according to values chosen from above, BUT the chosen attribute with random dummy value (that does not comply specification)
     -operation-key from above
     - reasonable parameters</v>
       </c>
@@ -4318,44 +4345,44 @@
 - searching CC for op-s of ",E3,", storing operation-key")
 &amp;CONCATENATE("
   - POST ",E3,"
-    - all attributes  filled with random dummy values  BUT application-release-number attribute with random dummy value differing from pattern in different ways
+    - all attributes filled with random dummy values  BUT application-release-number attribute with random dummy value differing from pattern in different ways
     -operation-key from above
     - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/disregard-application, storing operation-key
   - POST /v1/disregard-application
-    - all attributes  filled with random dummy values  BUT application-release-number attribute with random dummy value differing from pattern in different ways
+    - all attributes filled with random dummy values  BUT application-release-number attribute with random dummy value differing from pattern in different ways
     -operation-key from above
     - reasonable parameters</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G68" s="22" t="str">
         <f>CONCATENATE("#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
-- searching CC for op-s of ",G3,", storing operation-key- randomly choosing http-c from ltpList
-- Extracting authorization from config file")
+- searching CC for op-s of ",G3,", storing operation-key- randomly choosing http-c from ltpList")
 &amp;CONCATENATE("
   - POST ",G3,"
     - all attributes filled with chosen values  BUT application-release-number attribute with random dummy value differing from pattern in different ways
-    -operation-key from above
+    -operation-key from above, 
+- provide authorization from config file
     - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
 - searching CC for op-s of /v1/approve-oam-request, storing operation-key- randomly choosing http-c from ltpList
-- Extracting authorization from config file
   - POST /v1/approve-oam-request
     - all attributes filled with chosen values  BUT application-release-number attribute with random dummy value differing from pattern in different ways
-    -operation-key from above
+    -operation-key from above, 
+- provide authorization from config file
     - reasonable parameters</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="58"/>
+      <c r="A69" s="59"/>
       <c r="B69" s="8" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C69" s="50" t="s">
         <v>63</v>
@@ -4373,7 +4400,7 @@
 - verify that no changes happened on the configuration</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G69" s="26" t="str">
         <f>$C69</f>
@@ -4383,7 +4410,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="58"/>
+      <c r="A70" s="59"/>
       <c r="B70" s="8" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -4405,7 +4432,7 @@
 - not applicable</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G70" s="23" t="str">
         <f>$B19</f>
@@ -4414,7 +4441,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="58" t="s">
+      <c r="A71" s="59" t="s">
         <v>64</v>
       </c>
       <c r="B71" s="7" t="s">
@@ -4441,84 +4468,84 @@
         <v>## Get each attributes checked if getting correctly updated?</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="58"/>
+    <row r="72" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A72" s="59"/>
       <c r="B72" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>106</v>
+        <v>147</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="F72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G72" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="87" x14ac:dyDescent="0.35">
-      <c r="A73" s="58"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="59"/>
       <c r="B73" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>109</v>
+        <v>162</v>
       </c>
       <c r="E73" s="26" t="s">
-        <v>110</v>
+        <v>157</v>
       </c>
       <c r="F73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G73" s="26"/>
     </row>
-    <row r="74" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A74" s="58"/>
+    <row r="74" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="59"/>
       <c r="B74" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="D74" s="23" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="E74" s="23" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F74" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G74" s="23"/>
     </row>
     <row r="75" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="58"/>
+      <c r="A75" s="59"/>
       <c r="B75" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C75" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E75" s="25" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="G75" s="25"/>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="58" t="s">
-        <v>160</v>
+      <c r="A76" s="59" t="s">
+        <v>127</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>70</v>
@@ -4540,23 +4567,23 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" s="58"/>
+      <c r="A77" s="59"/>
       <c r="B77" s="12"/>
       <c r="C77" s="44" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E77" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="58"/>
+      <c r="A78" s="59"/>
       <c r="B78" s="8" t="s">
         <v>71</v>
       </c>
@@ -4571,50 +4598,50 @@
 - ExecutionAndTraceLog server to operate</v>
       </c>
       <c r="E78" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="58"/>
+      <c r="A79" s="59"/>
       <c r="B79" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="C79" s="46" t="s">
-        <v>157</v>
-      </c>
       <c r="D79" s="46" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="E79" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="58"/>
+      <c r="A80" s="59"/>
       <c r="B80" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D80" s="32" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="E80" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="58"/>
+      <c r="A81" s="59"/>
       <c r="B81" s="5" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -4631,14 +4658,14 @@
 - not applicable</v>
       </c>
       <c r="E81" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="58" t="s">
+      <c r="A82" s="59" t="s">
         <v>73</v>
       </c>
       <c r="B82" s="11" t="s">
@@ -4661,85 +4688,85 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="58"/>
+      <c r="A83" s="59"/>
       <c r="B83" s="13"/>
       <c r="C83" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D83" s="41" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E83" s="41" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F83" s="41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="58"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="261" x14ac:dyDescent="0.35">
+      <c r="A84" s="59"/>
       <c r="B84" s="12" t="s">
         <v>75</v>
       </c>
       <c r="C84" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="F84" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="116" x14ac:dyDescent="0.35">
-      <c r="A85" s="58"/>
+      <c r="A85" s="59"/>
       <c r="B85" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C85" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="E85" s="25" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="F85" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="58"/>
+      <c r="A86" s="59"/>
       <c r="B86" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C86" s="41"/>
       <c r="D86" s="23" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E86" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A87" s="58"/>
+      <c r="A87" s="59"/>
       <c r="B87" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C87" s="41"/>
       <c r="D87" s="25" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E87" s="25" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="58" t="s">
+      <c r="A88" s="59" t="s">
         <v>77</v>
       </c>
       <c r="B88" s="7" t="s">
@@ -4762,7 +4789,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A89" s="58"/>
+      <c r="A89" s="59"/>
       <c r="B89" s="8" t="s">
         <v>41</v>
       </c>
@@ -4773,78 +4800,78 @@
         <v>41</v>
       </c>
       <c r="E89" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F89" s="41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
-      <c r="A90" s="58"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="59"/>
       <c r="B90" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E90" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F90" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A91" s="58"/>
+      <c r="A91" s="59"/>
       <c r="B91" s="8" t="s">
         <v>80</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A92" s="58"/>
+      <c r="A92" s="59"/>
       <c r="B92" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="D92" s="23" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="58"/>
+      <c r="A93" s="59"/>
       <c r="B93" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C93" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D93" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="56"/>
+      <c r="A94" s="59"/>
       <c r="B94" s="8"/>
       <c r="C94" s="43" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D94" s="43" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A95" s="56"/>
+      <c r="A95" s="59"/>
       <c r="B95" s="8"/>
       <c r="C95" s="32" t="s">
         <v>41</v>
@@ -4854,7 +4881,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A96" s="60" t="s">
+      <c r="A96" s="62" t="s">
         <v>81</v>
       </c>
       <c r="B96" s="7" t="s">
@@ -4877,69 +4904,69 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" s="60"/>
+      <c r="A97" s="62"/>
       <c r="B97" s="8"/>
       <c r="C97" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D97" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E97" s="43" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F97" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A98" s="60"/>
+      <c r="A98" s="62"/>
       <c r="B98" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C98" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D98" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E98" s="32" t="s">
         <v>41</v>
       </c>
       <c r="F98" s="32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="261" x14ac:dyDescent="0.35">
-      <c r="A99" s="60"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="62"/>
       <c r="B99" s="8" t="s">
         <v>83</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D99" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E99" s="22" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="F99" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A100" s="60"/>
+      <c r="A100" s="62"/>
       <c r="B100" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C100" s="30"/>
       <c r="E100" s="26" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A101" s="60"/>
+      <c r="A101" s="62"/>
       <c r="B101" s="15" t="s">
         <v>49</v>
       </c>
@@ -4949,17 +4976,17 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A102" s="60"/>
+      <c r="A102" s="62"/>
       <c r="B102" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C102" s="30"/>
       <c r="E102" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A103" s="60" t="s">
+      <c r="A103" s="62" t="s">
         <v>85</v>
       </c>
       <c r="B103" s="7" t="s">
@@ -4982,73 +5009,73 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A104" s="60"/>
+      <c r="A104" s="62"/>
       <c r="B104" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C104" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D104" s="32" t="s">
         <v>41</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F104" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="60"/>
+      <c r="A105" s="62"/>
       <c r="B105" s="8" t="s">
         <v>83</v>
       </c>
       <c r="C105" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D105" s="22" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F105" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="60"/>
+      <c r="A106" s="62"/>
       <c r="B106" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C106" s="30"/>
       <c r="D106" s="26" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A107" s="60"/>
+      <c r="A107" s="62"/>
       <c r="B107" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C107" s="30"/>
       <c r="D107" s="23" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A108" s="60"/>
+      <c r="A108" s="62"/>
       <c r="B108" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C108" s="49"/>
       <c r="D108" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A109" s="60" t="s">
+      <c r="A109" s="62" t="s">
         <v>88</v>
       </c>
       <c r="B109" s="7" t="s">
@@ -5071,64 +5098,64 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A110" s="60"/>
+      <c r="A110" s="62"/>
       <c r="B110" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C110" s="48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D110" s="48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E110" s="48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F110" s="48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A111" s="60"/>
+      <c r="A111" s="62"/>
       <c r="B111" s="8" t="s">
         <v>83</v>
       </c>
       <c r="C111" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D111" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F111" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A112" s="60"/>
+      <c r="A112" s="62"/>
       <c r="B112" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C112" s="30"/>
     </row>
     <row r="113" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A113" s="60"/>
+      <c r="A113" s="62"/>
       <c r="B113" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C113" s="30"/>
     </row>
     <row r="114" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A114" s="60"/>
+      <c r="A114" s="62"/>
       <c r="B114" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C114" s="30"/>
     </row>
     <row r="115" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A115" s="60" t="s">
+      <c r="A115" s="62" t="s">
         <v>91</v>
       </c>
       <c r="B115" s="7" t="s">
@@ -5151,85 +5178,291 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A116" s="60"/>
+      <c r="A116" s="62"/>
       <c r="B116" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A117" s="59"/>
+      <c r="A117" s="61"/>
       <c r="B117" s="8" t="s">
         <v>83</v>
       </c>
       <c r="C117" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D117" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E117" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F117" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="145" x14ac:dyDescent="0.35">
-      <c r="A118" s="59"/>
+      <c r="A118" s="61"/>
       <c r="B118" s="8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A119" s="59"/>
+      <c r="A119" s="61"/>
       <c r="B119" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C119" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A120" s="59"/>
+      <c r="A120" s="61"/>
       <c r="B120" s="16" t="s">
         <v>54</v>
       </c>
       <c r="C120" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="59"/>
+      <c r="A121" s="61"/>
       <c r="C121" s="30"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A122" s="52"/>
-      <c r="C122" s="49"/>
+    <row r="122" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="57"/>
+      <c r="C122" s="56"/>
+    </row>
+    <row r="123" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="57"/>
+    </row>
+    <row r="124" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="57"/>
+    </row>
+    <row r="125" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="57"/>
+    </row>
+    <row r="126" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="57"/>
+    </row>
+    <row r="127" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="57"/>
+    </row>
+    <row r="128" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="57"/>
+    </row>
+    <row r="129" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="57"/>
+    </row>
+    <row r="130" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="57"/>
+    </row>
+    <row r="131" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="57"/>
+    </row>
+    <row r="132" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="57"/>
+    </row>
+    <row r="133" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="57"/>
+    </row>
+    <row r="134" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="57"/>
+    </row>
+    <row r="135" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="57"/>
+    </row>
+    <row r="136" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="57"/>
+    </row>
+    <row r="137" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="57"/>
+    </row>
+    <row r="138" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="57"/>
+    </row>
+    <row r="139" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="57"/>
+    </row>
+    <row r="140" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="57"/>
+    </row>
+    <row r="141" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="57"/>
+    </row>
+    <row r="142" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A142" s="57"/>
+    </row>
+    <row r="143" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="57"/>
+    </row>
+    <row r="144" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="57"/>
+    </row>
+    <row r="145" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="57"/>
+    </row>
+    <row r="146" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="57"/>
+    </row>
+    <row r="147" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="57"/>
+    </row>
+    <row r="148" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="57"/>
+    </row>
+    <row r="149" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="57"/>
+    </row>
+    <row r="150" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="57"/>
+    </row>
+    <row r="151" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="57"/>
+    </row>
+    <row r="152" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="57"/>
+    </row>
+    <row r="153" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="57"/>
+    </row>
+    <row r="154" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="57"/>
+    </row>
+    <row r="155" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="57"/>
+    </row>
+    <row r="156" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="57"/>
+    </row>
+    <row r="157" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="57"/>
+    </row>
+    <row r="158" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="57"/>
+    </row>
+    <row r="159" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="57"/>
+    </row>
+    <row r="160" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A160" s="57"/>
+    </row>
+    <row r="161" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="57"/>
+    </row>
+    <row r="162" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A162" s="57"/>
+    </row>
+    <row r="163" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="57"/>
+    </row>
+    <row r="164" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="57"/>
+    </row>
+    <row r="165" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="57"/>
+    </row>
+    <row r="166" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A166" s="57"/>
+    </row>
+    <row r="167" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A167" s="57"/>
+    </row>
+    <row r="168" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A168" s="57"/>
+    </row>
+    <row r="169" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A169" s="57"/>
+    </row>
+    <row r="170" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A170" s="57"/>
+    </row>
+    <row r="171" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A171" s="57"/>
+    </row>
+    <row r="172" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A172" s="57"/>
+    </row>
+    <row r="173" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A173" s="57"/>
+    </row>
+    <row r="174" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A174" s="57"/>
+    </row>
+    <row r="175" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A175" s="57"/>
+    </row>
+    <row r="176" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A176" s="57"/>
+    </row>
+    <row r="177" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A177" s="57"/>
+    </row>
+    <row r="178" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A178" s="57"/>
+    </row>
+    <row r="179" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A179" s="57"/>
+    </row>
+    <row r="180" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A180" s="57"/>
+    </row>
+    <row r="181" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="57"/>
+    </row>
+    <row r="182" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A182" s="57"/>
+    </row>
+    <row r="183" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A183" s="57"/>
+    </row>
+    <row r="184" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A184" s="57"/>
+    </row>
+    <row r="185" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A185" s="57"/>
+    </row>
+    <row r="186" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A186" s="57"/>
+    </row>
+    <row r="187" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A187" s="57"/>
+    </row>
+    <row r="188" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A188" s="57"/>
+    </row>
+    <row r="189" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A189" s="57"/>
+    </row>
+    <row r="190" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="57"/>
+    </row>
+    <row r="191" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A191" s="57"/>
+    </row>
+    <row r="192" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A192" s="57"/>
+    </row>
+    <row r="193" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A193" s="57"/>
+    </row>
+    <row r="194" spans="1:1" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A194" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A115:A121"/>
     <mergeCell ref="A59:A62"/>
@@ -5239,11 +5472,21 @@
     <mergeCell ref="A76:A81"/>
     <mergeCell ref="A82:A87"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A88:A93"/>
     <mergeCell ref="A96:A102"/>
     <mergeCell ref="A103:A108"/>
     <mergeCell ref="A109:A114"/>
     <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>